<commit_message>
Still can't figure out the problem statement
</commit_message>
<xml_diff>
--- a/CH-056 Process Efficiency.xlsx
+++ b/CH-056 Process Efficiency.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{886B34D9-1A39-4929-A309-112A91CA713E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4333420-64EA-4521-89E1-4D932BC6B4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4C27E944-9150-434A-ABF3-ACFF750898D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4C27E944-9150-434A-ABF3-ACFF750898D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Bo" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Bo!$B$2:$E$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$42</definedName>
   </definedNames>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="32">
   <si>
     <t>Result</t>
   </si>
@@ -1284,7 +1286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
     <sheetView workbookViewId="1">
@@ -2423,13 +2425,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43545E2-0A15-498A-94C8-3A483D2EB0F2}">
-  <dimension ref="B1:Q42"/>
+  <dimension ref="B1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="1">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3080,9 +3082,15 @@
         <v>12</v>
       </c>
       <c r="I23"/>
-      <c r="J23" s="5"/>
+      <c r="J23" s="5" cm="1">
+        <f t="array" ref="J23:J62">(E3:E42=_xlfn._xlws.SORT(_xlfn.UNIQUE(E3:E42)))*(C3:C42=_xlfn.UNIQUE(C3:C42))*(D3:D42=_xlfn.UNIQUE(D3:D42))</f>
+        <v>1</v>
+      </c>
       <c r="K23"/>
-      <c r="L23"/>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23:L26">_xlfn.UNIQUE(D3:D42)</f>
+        <v>3</v>
+      </c>
       <c r="M23"/>
       <c r="N23"/>
       <c r="O23"/>
@@ -3110,9 +3118,13 @@
         <v>7</v>
       </c>
       <c r="I24"/>
-      <c r="J24" s="5"/>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
       <c r="K24"/>
-      <c r="L24"/>
+      <c r="L24">
+        <v>2</v>
+      </c>
       <c r="M24"/>
       <c r="N24"/>
       <c r="O24"/>
@@ -3140,9 +3152,13 @@
         <v>6</v>
       </c>
       <c r="I25"/>
-      <c r="J25" s="5"/>
+      <c r="J25" s="5">
+        <v>0</v>
+      </c>
       <c r="K25"/>
-      <c r="L25"/>
+      <c r="L25">
+        <v>1</v>
+      </c>
       <c r="M25"/>
       <c r="N25"/>
       <c r="O25"/>
@@ -3170,9 +3186,13 @@
         <v>4</v>
       </c>
       <c r="I26"/>
-      <c r="J26" s="5"/>
+      <c r="J26" s="5">
+        <v>0</v>
+      </c>
       <c r="K26"/>
-      <c r="L26"/>
+      <c r="L26">
+        <v>4</v>
+      </c>
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -3200,7 +3220,9 @@
         <v>11</v>
       </c>
       <c r="I27"/>
-      <c r="J27" s="5"/>
+      <c r="J27" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -3226,7 +3248,9 @@
       <c r="G28" s="10"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28" s="5"/>
+      <c r="J28" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K28"/>
       <c r="L28"/>
       <c r="M28"/>
@@ -3252,7 +3276,9 @@
       <c r="G29" s="10"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29" s="5"/>
+      <c r="J29" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K29"/>
       <c r="L29"/>
       <c r="M29"/>
@@ -3278,7 +3304,9 @@
       <c r="G30" s="10"/>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30" s="5"/>
+      <c r="J30" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
@@ -3304,7 +3332,9 @@
       <c r="G31" s="10"/>
       <c r="H31"/>
       <c r="I31"/>
-      <c r="J31" s="5"/>
+      <c r="J31" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31"/>
@@ -3330,7 +3360,9 @@
       <c r="G32" s="10"/>
       <c r="H32"/>
       <c r="I32"/>
-      <c r="J32" s="5"/>
+      <c r="J32" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K32"/>
       <c r="L32"/>
       <c r="M32"/>
@@ -3356,7 +3388,9 @@
       <c r="G33" s="10"/>
       <c r="H33"/>
       <c r="I33"/>
-      <c r="J33" s="5"/>
+      <c r="J33" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
@@ -3382,7 +3416,9 @@
       <c r="G34" s="10"/>
       <c r="H34"/>
       <c r="I34"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K34"/>
       <c r="L34"/>
       <c r="M34"/>
@@ -3408,7 +3444,9 @@
       <c r="G35" s="10"/>
       <c r="H35"/>
       <c r="I35"/>
-      <c r="J35" s="5"/>
+      <c r="J35" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -3434,7 +3472,9 @@
       <c r="G36" s="10"/>
       <c r="H36"/>
       <c r="I36"/>
-      <c r="J36" s="5"/>
+      <c r="J36" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -3460,7 +3500,9 @@
       <c r="G37" s="10"/>
       <c r="H37"/>
       <c r="I37"/>
-      <c r="J37" s="5"/>
+      <c r="J37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -3486,7 +3528,9 @@
       <c r="G38" s="10"/>
       <c r="H38"/>
       <c r="I38"/>
-      <c r="J38" s="5"/>
+      <c r="J38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -3512,7 +3556,9 @@
       <c r="G39" s="10"/>
       <c r="H39"/>
       <c r="I39"/>
-      <c r="J39" s="5"/>
+      <c r="J39" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -3538,7 +3584,9 @@
       <c r="G40" s="10"/>
       <c r="H40"/>
       <c r="I40"/>
-      <c r="J40" s="5"/>
+      <c r="J40" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -3564,7 +3612,9 @@
       <c r="G41" s="10"/>
       <c r="H41"/>
       <c r="I41"/>
-      <c r="J41" s="5"/>
+      <c r="J41" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -3585,6 +3635,109 @@
       </c>
       <c r="E42" s="17" t="s">
         <v>20</v>
+      </c>
+      <c r="J42" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J43" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J48" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J50" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J62" s="5" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -3601,4 +3754,1198 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6BD4E4-0E6E-473D-A0EC-7579A5F658C2}">
+  <dimension ref="B1:Q42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="G1" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="33"/>
+      <c r="J1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>45305</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="18">
+        <v>3</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="19">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="26">
+        <v>0.09</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>45306</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="18">
+        <v>3</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="19">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="26">
+        <v>0.17</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>45306</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="19">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>45307</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="20">
+        <v>4</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0.33</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>45309</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4"/>
+      <c r="J7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <v>45311</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="25">
+        <v>3</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8" s="5"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>45311</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" s="5"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>45313</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10" s="5"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>45314</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11" s="5"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>45314</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="18">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="str" cm="1">
+        <f t="array" ref="G12:H16">_xlfn.LET(
+_xlpm.T,B3:E42,
+_xlpm.TT,G3:H6,
+_xlpm.P,_xlfn.CHOOSECOLS(_xlpm.T,2),
+_xlpm.PT,_xlfn.CHOOSECOLS(_xlpm.T,3),
+_xlpm.M,_xlfn.TAKE(_xlpm.T,,-1),
+_xlpm.PTT,_xlfn.TAKE(_xlpm.TT,,1),
+_xlpm.PTS,_xlfn.TAKE(_xlpm.TT,,-1),
+_xlpm.U,_xlfn.UNIQUE(_xlpm.P),
+_xlpm.XT,_xlfn.XLOOKUP(_xlpm.U,_xlpm.P,_xlpm.PT),
+_xlpm.MR,_xlfn.CONCAT(_xlfn.XLOOKUP(_xlpm.XT,_xlpm.PTT,_xlpm.PTS)),
+_xlpm.UU,_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.M)),
+_xlpm.R,_xlfn.MAP(_xlpm.UU,_xlfn.LAMBDA(_xlpm.A,_xlfn.LET(_xlpm.C,COUNTIFS(_xlpm.M,_xlpm.A),_xlpm.L,LEN(_xlpm.MR)-LEN(SUBSTITUTE(_xlpm.MR,_xlpm.A,"")),(_xlpm.C-_xlpm.L)/_xlpm.L))),
+_xlfn.HSTACK(_xlpm.UU,_xlpm.R)
+)</f>
+        <v>A</v>
+      </c>
+      <c r="H12">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12" s="5" t="str" cm="1">
+        <f t="array" ref="J12:J16">_xlfn.LET(
+_xlpm.T,B3:E42,
+_xlpm.TT,G3:H6,
+_xlpm.P,_xlfn.CHOOSECOLS(_xlpm.T,2),
+_xlpm.PT,_xlfn.CHOOSECOLS(_xlpm.T,3),
+_xlpm.M,_xlfn.TAKE(_xlpm.T,,-1),
+_xlpm.PTT,_xlfn.TAKE(_xlpm.TT,,1),
+_xlpm.PTS,_xlfn.TAKE(_xlpm.TT,,-1),
+_xlpm.U,_xlfn.UNIQUE(_xlpm.P),
+_xlpm.XT,_xlfn.XLOOKUP(_xlpm.U,_xlpm.P,_xlpm.PT),
+_xlpm.MR,_xlfn.CONCAT(_xlfn.XLOOKUP(_xlpm.XT,_xlpm.PTT,_xlpm.PTS)),
+_xlpm.UU,_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlpm.M)),
+_xlpm.R,_xlfn.MAP(_xlpm.UU,_xlfn.LAMBDA(_xlpm.A,_xlfn.LET(_xlpm.C,COUNTIFS(_xlpm.M,_xlpm.A),_xlpm.L,LEN(_xlpm.MR)-LEN(SUBSTITUTE(_xlpm.MR,_xlpm.A,"")),(_xlpm.C-_xlpm.L)/_xlpm.L))),
+_xlpm.UU
+)</f>
+        <v>A</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23">
+        <v>45318</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="str">
+        <v>B</v>
+      </c>
+      <c r="H13">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="18">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="str">
+        <v>C</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14" s="5" t="str">
+        <v>C</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="str">
+        <v>D</v>
+      </c>
+      <c r="H15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15" s="5" t="str">
+        <v>D</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="18">
+        <v>2</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="str">
+        <v>E</v>
+      </c>
+      <c r="H16">
+        <v>0.1</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16" s="5" t="str">
+        <v>E</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <v>45320</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17" s="5"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <v>45321</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18" s="5"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>45321</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="18">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19" s="5"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>45322</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20" s="5"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23">
+        <v>45322</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="25">
+        <v>2</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21" s="5"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>45323</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="18">
+        <v>1</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22" s="5"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
+        <v>45324</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="18">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23" s="5"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>45325</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="18">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24" s="5"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
+        <v>45325</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="18">
+        <v>3</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25" s="5"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>45326</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="18">
+        <v>4</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26" s="5"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
+        <v>45327</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="18">
+        <v>2</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27" s="5"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
+        <v>45327</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28" s="5"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="23">
+        <v>45328</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="25">
+        <v>1</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29" s="5"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
+        <v>45328</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="18">
+        <v>2</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="5"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="16">
+        <v>45328</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="18">
+        <v>2</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31" s="5"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="16">
+        <v>45330</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="18">
+        <v>2</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32" s="5"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="16">
+        <v>45332</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="18">
+        <v>3</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" s="5"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="16">
+        <v>45332</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="18">
+        <v>2</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34" s="5"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="16">
+        <v>45334</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="18">
+        <v>1</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35" s="5"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="16">
+        <v>45336</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36" s="5"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+    </row>
+    <row r="37" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="16">
+        <v>45336</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="18">
+        <v>2</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37" s="5"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+    </row>
+    <row r="38" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="16">
+        <v>45337</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38" s="5"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+    </row>
+    <row r="39" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="16">
+        <v>45341</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39" s="5"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+    </row>
+    <row r="40" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="16">
+        <v>45345</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="18">
+        <v>2</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40" s="5"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+    </row>
+    <row r="41" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="16">
+        <v>45352</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="18">
+        <v>2</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41" s="5"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="16">
+        <v>45356</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="18">
+        <v>2</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:E42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I think I now have a good description
</commit_message>
<xml_diff>
--- a/CH-056 Process Efficiency.xlsx
+++ b/CH-056 Process Efficiency.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A1532E-56D6-4C21-A9F8-44B087E2B5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D95E4DD-0B4D-4A27-8794-C5C679CDF86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4C27E944-9150-434A-ABF3-ACFF750898D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{4C27E944-9150-434A-ABF3-ACFF750898D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Bo" sheetId="3" r:id="rId3"/>
+    <sheet name="EDA2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Bo!$B$2:$E$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EDA2'!$B$2:$E$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="33">
   <si>
     <t>Result</t>
   </si>
@@ -161,6 +163,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Fault</t>
   </si>
 </sst>
 </file>
@@ -545,6 +550,15 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,22 +571,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1732,20 +1752,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="G1" s="34" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="H1" s="38"/>
+      <c r="J1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -2912,7 +2932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43545E2-0A15-498A-94C8-3A483D2EB0F2}">
   <dimension ref="B1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I6" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -2932,20 +2952,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="G1" s="34" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="H1" s="38"/>
+      <c r="J1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -2973,7 +2993,7 @@
       <c r="K2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="32" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3005,7 +3025,7 @@
       </c>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="33" t="s">
         <v>2</v>
       </c>
       <c r="O3" s="12"/>
@@ -3040,7 +3060,7 @@
       </c>
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="34" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="12"/>
@@ -3075,7 +3095,7 @@
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="33" t="s">
         <v>20</v>
       </c>
       <c r="O5" s="12"/>
@@ -3110,7 +3130,7 @@
       </c>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="33" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="12"/>
@@ -4271,20 +4291,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="G1" s="34" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="J1" s="34" t="s">
+      <c r="H1" s="38"/>
+      <c r="J1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="35"/>
+      <c r="K1" s="38"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -5438,4 +5458,1361 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4040AF29-AD88-4777-8B8B-C57D4FD8F8DC}">
+  <dimension ref="B1:Q42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.19921875" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.8984375" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.8984375" customWidth="1"/>
+    <col min="18" max="18" width="17.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="G1" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="38"/>
+      <c r="J1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>45305</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="18">
+        <v>3</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="26">
+        <v>0.09</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="10"/>
+    </row>
+    <row r="4" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>45306</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="18">
+        <v>3</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="26">
+        <v>0.17</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>45306</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>45307</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="20">
+        <v>4</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0.33</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>45309</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4"/>
+      <c r="J7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <v>45311</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="25">
+        <v>3</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8" s="5"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16">
+        <v>45311</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10">
+        <v>7</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" s="5"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
+        <v>45313</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="18">
+        <v>2</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" aca="1" ref="L10" ca="1">_xlfn.XLOOKUP(0,_xlfn.ANCHORARRAY(G16),OFFSET(I16,0,0,ROWS(_xlfn.ANCHORARRAY(H16))),1)</f>
+        <v>6</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10" s="31"/>
+    </row>
+    <row r="11" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>45314</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>9</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11" s="5"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11" s="31"/>
+    </row>
+    <row r="12" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>45314</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="18">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="5" t="str">
+        <f>J23</f>
+        <v>PI-063</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12" s="5"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12" s="31"/>
+    </row>
+    <row r="13" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23">
+        <v>45318</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>11</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13:I13">MID(H12,{1,6},{5,1})</f>
+        <v>PI-06</v>
+      </c>
+      <c r="I13" t="str">
+        <v>3</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13" s="31"/>
+    </row>
+    <row r="14" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="18">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10">
+        <v>12</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14" s="5"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14" s="31"/>
+    </row>
+    <row r="15" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="18">
+        <v>2</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15" s="5"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
+        <v>45319</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="18">
+        <v>2</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" cm="1">
+        <f t="array" ref="G16:G18">--(_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(H16),1)=_xlfn.ANCHORARRAY(K16))</f>
+        <v>1</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16:I18">_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER(B3:F42,H13=_xlfn.CHOOSECOLS(B3:E42,2)),4,5)</f>
+        <v>A</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" t="str" cm="1">
+        <f t="array" ref="K16:K18">_xlfn.EXPAND(_xlfn.TEXTSPLIT(_xlfn.XLOOKUP(I13+0,G3:G6,H3:H6),,",",TRUE),ROWS(_xlfn.ANCHORARRAY(H16)),1,"x")</f>
+        <v>A</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
+        <v>45320</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10">
+        <v>15</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <v>E</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" t="str">
+        <v>E</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
+        <v>45321</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="18">
+        <v>4</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>16</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" t="str">
+        <v>E</v>
+      </c>
+      <c r="I18" s="1">
+        <v>6</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" t="str">
+        <v>x</v>
+      </c>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
+        <v>45321</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="18">
+        <v>2</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="10">
+        <v>17</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19"/>
+      <c r="J19" s="5"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
+        <v>45322</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="10">
+        <v>18</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20"/>
+      <c r="J20" s="5"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="23">
+        <v>45322</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="25">
+        <v>2</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10">
+        <v>19</v>
+      </c>
+      <c r="G21" s="10"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21" s="5"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>45323</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="18">
+        <v>1</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="10">
+        <v>20</v>
+      </c>
+      <c r="I22"/>
+      <c r="J22" s="5"/>
+      <c r="K22">
+        <f ca="1">L10</f>
+        <v>6</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
+        <v>45324</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="18">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="10">
+        <v>21</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" t="str" cm="1">
+        <f t="array" ref="H23:I32">_xlfn.UNIQUE(C3:D42)</f>
+        <v>PI-06</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23" s="5" t="str" cm="1">
+        <f t="array" ref="J23:J32">_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(H23),1)&amp;_xlfn.CHOOSECOLS(_xlfn.ANCHORARRAY(H23),2)</f>
+        <v>PI-063</v>
+      </c>
+      <c r="K23">
+        <f t="dataTable" ref="K23:K32" dt2D="0" dtr="0" r1="H12" ca="1"/>
+        <v>6</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>45325</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="18">
+        <v>1</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="10">
+        <v>22</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" t="str">
+        <v>PI-07</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24" s="5" t="str">
+        <v>PI-073</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+    </row>
+    <row r="25" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
+        <v>45325</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="18">
+        <v>3</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>23</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" t="str">
+        <v>PI-17</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25" s="5" t="str">
+        <v>PI-172</v>
+      </c>
+      <c r="K25">
+        <v>19</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>45326</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="18">
+        <v>4</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>24</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" t="str">
+        <v>PI-15</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5" t="str">
+        <v>PI-151</v>
+      </c>
+      <c r="K26">
+        <v>11</v>
+      </c>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
+        <v>45327</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="18">
+        <v>2</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="10">
+        <v>25</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" t="str">
+        <v>PI-05</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5" t="str">
+        <v>PI-051</v>
+      </c>
+      <c r="K27">
+        <v>27</v>
+      </c>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+    </row>
+    <row r="28" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
+        <v>45327</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="18">
+        <v>1</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="10">
+        <v>26</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" t="str">
+        <v>PI-10</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28" s="5" t="str">
+        <v>PI-102</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="23">
+        <v>45328</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="25">
+        <v>1</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10">
+        <v>27</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" t="str">
+        <v>PI-14</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29" s="5" t="str">
+        <v>PI-144</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
+        <v>45328</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="18">
+        <v>2</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="10">
+        <v>28</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" t="str">
+        <v>PI-01</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5" t="str">
+        <v>PI-011</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+    </row>
+    <row r="31" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="16">
+        <v>45328</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="18">
+        <v>2</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="10">
+        <v>29</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" t="str">
+        <v>PI-09</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31" s="5" t="str">
+        <v>PI-093</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="16">
+        <v>45330</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="18">
+        <v>2</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="10">
+        <v>30</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" t="str">
+        <v>PI-16</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" s="5" t="str">
+        <v>PI-162</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="16">
+        <v>45332</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="18">
+        <v>3</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="10">
+        <v>31</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" s="5"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="16">
+        <v>45332</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="18">
+        <v>2</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <v>32</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34" s="5"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="16">
+        <v>45334</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="18">
+        <v>1</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="10">
+        <v>33</v>
+      </c>
+      <c r="G35" s="10"/>
+      <c r="H35"/>
+      <c r="I35" cm="1">
+        <f t="array" ref="I35:I38">_xlfn._xlws.FILTER(K23:K32,K23:K32&lt;&gt;1)</f>
+        <v>6</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="16">
+        <v>45336</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="18">
+        <v>1</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="10">
+        <v>34</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36"/>
+      <c r="I36">
+        <v>19</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+    </row>
+    <row r="37" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="16">
+        <v>45336</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="18">
+        <v>2</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="10">
+        <v>35</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37"/>
+      <c r="I37">
+        <v>11</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+    </row>
+    <row r="38" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="16">
+        <v>45337</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="18">
+        <v>1</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="10">
+        <v>36</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38"/>
+      <c r="I38">
+        <v>27</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+    </row>
+    <row r="39" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="16">
+        <v>45341</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="18">
+        <v>1</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="10">
+        <v>37</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39" s="5"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+    </row>
+    <row r="40" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="16">
+        <v>45345</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="18">
+        <v>2</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="10">
+        <v>38</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40" s="5"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+    </row>
+    <row r="41" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="16">
+        <v>45352</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="18">
+        <v>2</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="10">
+        <v>39</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41" s="5"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="16">
+        <v>45356</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="18">
+        <v>2</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="10">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:E42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>H21&lt;&gt;I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:H20">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>H16&lt;&gt;K16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Intermediate result toward a single function
</commit_message>
<xml_diff>
--- a/CH-056 Process Efficiency.xlsx
+++ b/CH-056 Process Efficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="346" documentId="8_{568298C5-F349-41B3-BA30-1EA8ED577E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F30EA94F-1ED7-4D73-81D2-8527E08794D8}"/>
+  <xr:revisionPtr revIDLastSave="348" documentId="8_{568298C5-F349-41B3-BA30-1EA8ED577E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F833B40-2F61-4D51-AFAB-6FDF7CF7A09C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{4C27E944-9150-434A-ABF3-ACFF750898D8}"/>
   </bookViews>
@@ -595,6 +595,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -606,13 +613,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1795,20 +1795,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -2995,20 +2995,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -4334,20 +4334,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -5508,7 +5508,7 @@
   <dimension ref="B1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47:H51"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5533,20 +5533,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -6942,7 +6942,7 @@
       <c r="F47">
         <v>3</v>
       </c>
-      <c r="H47" s="40" cm="1">
+      <c r="H47" s="36" cm="1">
         <f t="array" ref="H47:H51">_xlfn.LET(_xlpm.fm, _xlfn.LAMBDA(_xlpm.qq,_xlfn.LET(
 _xlpm.k,_xlfn.UNIQUE($C$3:$D$42),
 _xlpm.fn,_xlfn.LAMBDA(_xlpm.ke,_xlfn.LET(_xlpm.x,_xlfn.XLOOKUP(INDEX(_xlpm.ke,,2),$G$3:$G$6,$H$3:$H$6),_xlfn.TEXTSPLIT(_xlpm.x,,","))),
@@ -6958,7 +6958,7 @@
 )</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="K47" s="41" t="s">
+      <c r="K47" s="37" t="s">
         <v>38</v>
       </c>
     </row>
@@ -6983,7 +6983,7 @@
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="J49" s="42" t="s">
+      <c r="J49" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -7097,20 +7097,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="G1" s="38" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="J1" s="38" t="s">
+      <c r="H1" s="42"/>
+      <c r="J1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="39"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">

</xml_diff>